<commit_message>
Fixed stage_one: quantitative and qualitative tests are generated correctly; Fixed stage_two: implemented required improvements;
</commit_message>
<xml_diff>
--- a/resources/autotests.xlsx
+++ b/resources/autotests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\forecast-autotests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A958E45-7EEE-4812-8582-4CF2F7544C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428FEB0D-08E7-4076-85B1-EC7A792B4947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2355" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9C7392BA-0153-4ED4-B1EE-FAC0C59CC996}"/>
+    <workbookView xWindow="8970" yWindow="4215" windowWidth="29430" windowHeight="15345" activeTab="1" xr2:uid="{9C7392BA-0153-4ED4-B1EE-FAC0C59CC996}"/>
   </bookViews>
   <sheets>
     <sheet name="Список качественных автотестов" sheetId="1" r:id="rId1"/>
@@ -610,9 +610,6 @@
     <t>2025;2027</t>
   </si>
   <si>
-    <t>Год запуска</t>
-  </si>
-  <si>
     <t>Эффект за 2025-2026 года по tNav</t>
   </si>
   <si>
@@ -728,6 +725,9 @@
   </si>
   <si>
     <t xml:space="preserve">Интегральный эффект уменьшается в сравнении с id№1, так более позднее внедрение мероприятия означает более низкое пластовое давление в год проведения мероприятия. </t>
+  </si>
+  <si>
+    <t>Год запуска</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1449,7 @@
         <v>93</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>36</v>
@@ -1474,7 +1474,7 @@
         <v>96</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>37</v>
@@ -1562,7 +1562,7 @@
         <v>103</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>102</v>
@@ -1603,10 +1603,10 @@
         <v>94</v>
       </c>
       <c r="E10" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="29" t="s">
         <v>221</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>222</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>36</v>
@@ -1627,10 +1627,10 @@
         <v>95</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>37</v>
@@ -1695,10 +1695,10 @@
         <v>115</v>
       </c>
       <c r="E14" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="29" t="s">
         <v>218</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>219</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>102</v>
@@ -1763,10 +1763,10 @@
         <v>122</v>
       </c>
       <c r="E17" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="F17" s="29" t="s">
         <v>216</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>217</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>102</v>
@@ -1831,10 +1831,10 @@
         <v>122</v>
       </c>
       <c r="E20" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>214</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>215</v>
       </c>
       <c r="G20" s="29" t="s">
         <v>102</v>
@@ -1899,10 +1899,10 @@
         <v>122</v>
       </c>
       <c r="E23" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="F23" s="29" t="s">
         <v>212</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>213</v>
       </c>
       <c r="G23" s="29" t="s">
         <v>102</v>
@@ -1967,10 +1967,10 @@
         <v>131</v>
       </c>
       <c r="E26" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="F26" s="29" t="s">
         <v>210</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>211</v>
       </c>
       <c r="G26" s="29" t="s">
         <v>102</v>
@@ -2035,10 +2035,10 @@
         <v>131</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G29" s="29" t="s">
         <v>102</v>
@@ -2103,10 +2103,10 @@
         <v>131</v>
       </c>
       <c r="E32" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="F32" s="29" t="s">
         <v>206</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>207</v>
       </c>
       <c r="G32" s="29" t="s">
         <v>102</v>
@@ -2171,10 +2171,10 @@
         <v>131</v>
       </c>
       <c r="E35" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F35" s="29" t="s">
         <v>204</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>205</v>
       </c>
       <c r="G35" s="29" t="s">
         <v>102</v>
@@ -2218,7 +2218,7 @@
         <v>145</v>
       </c>
       <c r="F37" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G37" s="29" t="s">
         <v>36</v>
@@ -2239,10 +2239,10 @@
         <v>131</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G38" s="29" t="s">
         <v>102</v>
@@ -2307,10 +2307,10 @@
         <v>131</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G41" s="29" t="s">
         <v>102</v>
@@ -2351,10 +2351,10 @@
         <v>130</v>
       </c>
       <c r="E43" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="29" t="s">
         <v>197</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>198</v>
       </c>
       <c r="G43" s="29" t="s">
         <v>36</v>
@@ -2375,10 +2375,10 @@
         <v>131</v>
       </c>
       <c r="E44" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="F44" s="29" t="s">
         <v>195</v>
-      </c>
-      <c r="F44" s="29" t="s">
-        <v>196</v>
       </c>
       <c r="G44" s="29" t="s">
         <v>102</v>
@@ -2443,10 +2443,10 @@
         <v>131</v>
       </c>
       <c r="E47" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F47" s="29" t="s">
         <v>193</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>194</v>
       </c>
       <c r="G47" s="29" t="s">
         <v>102</v>
@@ -2511,10 +2511,10 @@
         <v>161</v>
       </c>
       <c r="E50" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" s="29" t="s">
         <v>191</v>
-      </c>
-      <c r="F50" s="29" t="s">
-        <v>192</v>
       </c>
       <c r="G50" s="29" t="s">
         <v>112</v>
@@ -2526,7 +2526,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C51" s="28" t="s">
         <v>177</v>
@@ -2706,7 +2706,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2727,13 +2727,13 @@
         <v>10</v>
       </c>
       <c r="C1" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="E1" s="44" t="s">
         <v>188</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>189</v>
       </c>
       <c r="F1" s="44" t="s">
         <v>38</v>
@@ -2753,8 +2753,14 @@
       <c r="D2">
         <v>-12976245248</v>
       </c>
+      <c r="E2">
+        <v>-20006000</v>
+      </c>
       <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="G2" s="39">
+        <f>(1-(D2-E2)/D2)*100</f>
+        <v>0.1541740281387094</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="37">
@@ -3166,7 +3172,7 @@
   </sheetPr>
   <dimension ref="B1:AC1006"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>